<commit_message>
Issue #18 WebSocket 필요 항목 중 다음과 같은 항목 완료 - WebSocket용 Communicator 작성하기 - Communicator Parent Class 작성하기 - WebSocket용 / 일반 Socket용 분리해서 사용할 수 있게 하기
</commit_message>
<xml_diff>
--- a/CommunicationSpec.xlsx
+++ b/CommunicationSpec.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROJECT\UnityProject\PROJECT\UnityOnlineProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12925E2-76B8-4CD8-A20E-3971628BE7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76BE576-9073-4A67-ABC6-137663E3BD34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8190" yWindow="5640" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{C4C8D13A-16D1-42DF-AF52-E4B8468C6B80}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15345" xr2:uid="{C4C8D13A-16D1-42DF-AF52-E4B8468C6B80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$C$3:$C$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$C$3:$C$6</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="122">
   <si>
     <t>프로토콜 일람</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -203,34 +204,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SOF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EOF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>데이터 프레임 구조</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>JSON Data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data with JSON</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GameObjectSpawnReport</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -326,6 +303,282 @@
   </si>
   <si>
     <t>플레이어의 요청에 대한 응답</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WebSocket RFC6455사양을 따름 (https://www.rfc-editor.org/rfc/rfc6455#section-1.2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RSV1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RSV2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RSV3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1Byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OpCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뒤에서 이어지는 프레임</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>텍스트 프레임</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000 (0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001 (1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0010 (2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바이너리 프레임</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000 (8)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연결 종료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1001 (9)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>핑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1010 (A)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>퐁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기재하지 않은 다른거</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Custom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2Byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MASK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>특별히 정한게 없으면 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0bX0000000 (0)
+~
+0bX1111111(127)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Masking
+Key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2번째 Byte의 MASK가 1이라면 사용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3Byte
+~
+10Byte
+(8Byte)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">11Byte
+~
+14Byte
+(4Byte)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0이면 즉시 데이터로 시작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세 개 중에 하나만 가능하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이후 데이터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공식에서 제시한 예시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프레임 끝(프레임의 끝을 담당하며, 자동으로 시작도 담당하게 됨). Countinous Frame의 경우엔 0이어야 함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WebSocket RFC 6455 Spec Case</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Case 1 : 한번에 데이터가 몰려 프레임이 분리됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0b00000001 0x03 0x48 0x65 0x6c (contains "Hel")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0b10000000 0x02 0x6c 0x6f (contains "lo")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RCV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1st</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2nd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마스킹 설정. 클라이언트는 서버에게 마스킹된 데이터를 보내야만 함. 마스킹되지 않은 데이터를 서버가 받으면 1002번 (프로토콜 에러) 오류를 발송할 것</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Case 2 : 데이터가 깨짐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-&gt; 여기서부터 이전 데이터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Case 3 : 이전 데이터가 남음 -&gt; 처리하면서 0으로 비우는 로직 사용하면 없앨 수 있음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-&gt; 여기서부터 다시 시작 / 어떻게 분간할 것인지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x89 0x05 0x48 0x65 0x6c 0x6c 0x6f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0b10001001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ping</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ContinuousData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>위에서부터 7번째 bit -&gt; 0번째 bit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0b00000000 (0)
+~
+0b11111111(255)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ex) 0x82 0x7E 0x01 0x00 Data…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unmasked Frame</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x7E = 0b01111110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01 = 0b00000001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>따라서,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7 (125까지) / 7 + 16 / 7 + 64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>126인 경우, 다음 2Byte가 길이가 된다. 127인 경우, 다음 8byte가 길이이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIN은 1이고, OPCode는 Continuous</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIN은 0이고, OPCode는 …</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -388,7 +641,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -407,7 +660,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -432,23 +685,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -764,68 +1047,634 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8053D23-4EB6-4ED3-B75B-64D93E2A5E34}">
-  <dimension ref="B2:G7"/>
+  <dimension ref="B2:I48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="9" style="8" customWidth="1"/>
+    <col min="4" max="4" width="20.625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="30.625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="20.625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="30.625" customWidth="1"/>
+    <col min="8" max="9" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="18"/>
+      <c r="C8" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="16">
+        <v>0</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="18"/>
+      <c r="C9" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0</v>
+      </c>
+      <c r="E9" s="17"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="18"/>
+      <c r="C10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0</v>
+      </c>
+      <c r="E10" s="17"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="18"/>
+      <c r="C16" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="20"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="19"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="19"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="19"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="19"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="19"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="19"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="19"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B31" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="E32" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="10"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B44" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="F44" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="G44" s="12"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B45" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="F45" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G45" s="12"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B46" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B47" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B48" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B31:B38"/>
+    <mergeCell ref="C31:C38"/>
+    <mergeCell ref="C23:C30"/>
+    <mergeCell ref="D23:D30"/>
+    <mergeCell ref="B15:B22"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="C16:C22"/>
+    <mergeCell ref="D16:D22"/>
+    <mergeCell ref="B23:B30"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B7:B14"/>
+    <mergeCell ref="C11:C14"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4BCD7E5-B0CA-440C-BDBF-5E721E16F3D5}">
+  <dimension ref="B3:X19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" t="s">
-        <v>33</v>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B7" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="18"/>
+      <c r="V7" s="18"/>
+      <c r="W7" s="18"/>
+      <c r="X7" s="3"/>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" t="s">
+        <v>57</v>
+      </c>
+      <c r="K8" t="s">
+        <v>97</v>
+      </c>
+      <c r="L8" t="s">
+        <v>79</v>
+      </c>
+      <c r="M8" t="s">
+        <v>81</v>
+      </c>
+      <c r="N8" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="3"/>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="M9" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B12" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" t="s">
+        <v>97</v>
+      </c>
+      <c r="I13" t="s">
+        <v>79</v>
+      </c>
+      <c r="J13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" t="s">
+        <v>97</v>
+      </c>
+      <c r="L18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J19" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="C7:F7"/>
+  <mergeCells count="7">
+    <mergeCell ref="M7:W7"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="B12:L12"/>
+    <mergeCell ref="B17:L17"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="B7:L7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD5444D-5353-498B-B134-3C7F6C4BB98B}">
   <dimension ref="B2:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -869,10 +1718,10 @@
       <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="11"/>
+      <c r="G3" s="23"/>
       <c r="H3" s="2" t="s">
         <v>17</v>
       </c>
@@ -931,23 +1780,23 @@
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
         <v>51</v>
       </c>
-      <c r="F7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" t="s">
-        <v>57</v>
-      </c>
       <c r="H7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
@@ -959,64 +1808,64 @@
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="17"/>
+      <c r="F11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="17"/>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="10"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="10"/>
-      <c r="F11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" t="s">
-        <v>57</v>
-      </c>
-      <c r="H11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="10"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="10"/>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" t="s">
         <v>54</v>
       </c>
-      <c r="G12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" t="s">
-        <v>56</v>
-      </c>
-      <c r="I12" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="10"/>
-      <c r="C13" s="9"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="10"/>
+      <c r="E13" s="17"/>
       <c r="F13" t="s">
         <v>20</v>
       </c>
@@ -1027,14 +1876,14 @@
         <v>19</v>
       </c>
       <c r="I13" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="10"/>
-      <c r="C14" s="9"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="10"/>
+      <c r="E14" s="17"/>
       <c r="F14" t="s">
         <v>21</v>
       </c>
@@ -1054,30 +1903,30 @@
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>43</v>
-      </c>
       <c r="D17" s="7"/>
-      <c r="E17" s="13" t="s">
-        <v>45</v>
+      <c r="E17" s="22" t="s">
+        <v>39</v>
       </c>
       <c r="F17" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G17" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H17" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="10"/>
-      <c r="C18" s="9"/>
-      <c r="E18" s="13"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="E18" s="22"/>
       <c r="F18" t="s">
         <v>20</v>
       </c>
@@ -1092,9 +1941,9 @@
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
-      <c r="C19" s="9"/>
-      <c r="E19" s="13"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="E19" s="22"/>
       <c r="F19" t="s">
         <v>21</v>
       </c>
@@ -1106,9 +1955,9 @@
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="10"/>
-      <c r="C20" s="9"/>
-      <c r="E20" s="13"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="E20" s="22"/>
       <c r="F20" t="s">
         <v>23</v>
       </c>
@@ -1119,13 +1968,13 @@
         <v>22</v>
       </c>
       <c r="I20" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="10"/>
-      <c r="C21" s="9"/>
-      <c r="E21" s="13"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="E21" s="22"/>
       <c r="F21" t="s">
         <v>24</v>
       </c>
@@ -1141,58 +1990,58 @@
     </row>
     <row r="23" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>46</v>
+        <v>38</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G23" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H23" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E24" s="13"/>
+      <c r="E24" s="22"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E25" s="12"/>
+      <c r="E25" s="9"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E26" s="12"/>
+      <c r="E26" s="9"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E27" s="12"/>
+      <c r="E27" s="9"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>48</v>
+        <v>38</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>42</v>
       </c>
       <c r="F29" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G29" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H29" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E30" s="13"/>
+      <c r="E30" s="22"/>
       <c r="F30" t="s">
         <v>20</v>
       </c>
@@ -1204,7 +2053,7 @@
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E31" s="13"/>
+      <c r="E31" s="22"/>
       <c r="F31" t="s">
         <v>21</v>
       </c>
@@ -1216,7 +2065,7 @@
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E32" s="13"/>
+      <c r="E32" s="22"/>
       <c r="F32" t="s">
         <v>23</v>
       </c>
@@ -1228,7 +2077,7 @@
       </c>
     </row>
     <row r="33" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E33" s="13"/>
+      <c r="E33" s="22"/>
       <c r="F33" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Issue #22 Skill 시스템 완료
Issue #21 발사체 및 상호작용 추가 중 다음과 같은 항목 완료
- Fire하면 발사체 추가하기 -> 새로운 Issue (Skill System)
- 발사체를 추가할 때, 모두에게 발신
- 발사체 발사 메시지 발신시, 발사체의 힘도 발신
- 발사체 발사 및 힘을 수신한 플레이어의 클라이언트에 객체 추가 및 힘 추가
</commit_message>
<xml_diff>
--- a/CommunicationSpec.xlsx
+++ b/CommunicationSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROJECT\UnityProject\PROJECT\UnityOnlineProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3A22F6-EE6D-41C3-9E4D-1C2BA709BF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B18822E-D3AB-411E-A6F8-C9B1983C805C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="2970" windowWidth="25845" windowHeight="17715" xr2:uid="{C4C8D13A-16D1-42DF-AF52-E4B8468C6B80}"/>
+    <workbookView xWindow="2220" yWindow="1515" windowWidth="25845" windowHeight="17715" activeTab="1" xr2:uid="{C4C8D13A-16D1-42DF-AF52-E4B8468C6B80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="138">
   <si>
     <t>프로토콜 일람</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -222,18 +222,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>GameObjectSpawnRequest</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>C → S</t>
   </si>
   <si>
     <t>플레이어가 자신의 GameObject를 요청함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GameObjectSpawnRequest (Reply)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -594,6 +586,61 @@
   </si>
   <si>
     <t>0x00000000 ~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlayerTankSpawnRequest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlayerTankSpawnRequest (Reply)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameObjectSpawnReport</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새로운 GameObject Spawn 안내</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Force</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BulletSpawnRequest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>힘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>["Force"] = "1,00, 1.001, 1.002, 1.003"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bullet 생성 요청. 힘 또한 주어 즉시 사용할 수 있게 함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>["ObjectType"] = "Bullet"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>["ObjectSubType"] = "Normal"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bullet의 주인 객체</t>
+  </si>
+  <si>
+    <t>["ID"] = "1111"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -675,7 +722,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -742,14 +789,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1073,7 +1132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8053D23-4EB6-4ED3-B75B-64D93E2A5E34}">
   <dimension ref="B2:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
@@ -1089,18 +1148,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="15"/>
@@ -1109,363 +1168,368 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="21" t="s">
-        <v>52</v>
+      <c r="B7" s="25" t="s">
+        <v>50</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="21"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D8" s="16">
         <v>0</v>
       </c>
-      <c r="E8" s="23" t="s">
-        <v>71</v>
+      <c r="E8" s="24" t="s">
+        <v>69</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="21"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D9" s="16">
         <v>0</v>
       </c>
-      <c r="E9" s="23"/>
+      <c r="E9" s="24"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="21"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D10" s="16">
         <v>0</v>
       </c>
-      <c r="E10" s="23"/>
+      <c r="E10" s="24"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="21"/>
-      <c r="C11" s="21" t="s">
+      <c r="B11" s="25"/>
+      <c r="C11" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="F12" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E13" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="G13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="8" t="s">
+      <c r="E15" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="25"/>
+      <c r="C16" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="21"/>
-      <c r="C16" s="21" t="s">
+      <c r="D16" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="27"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="26"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="26"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B31" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="24"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="22"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B39" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B43" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C43" s="10"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B44" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
       <c r="F44" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G44" s="12"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B45" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
       <c r="F45" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G45" s="12"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B46" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B47" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B48" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B31:B38"/>
+    <mergeCell ref="C31:C38"/>
+    <mergeCell ref="C23:C30"/>
+    <mergeCell ref="D23:D30"/>
+    <mergeCell ref="B15:B22"/>
     <mergeCell ref="E8:E10"/>
     <mergeCell ref="C16:C22"/>
     <mergeCell ref="D16:D22"/>
@@ -1473,11 +1537,6 @@
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B7:B14"/>
     <mergeCell ref="C11:C14"/>
-    <mergeCell ref="B31:B38"/>
-    <mergeCell ref="C31:C38"/>
-    <mergeCell ref="C23:C30"/>
-    <mergeCell ref="D23:D30"/>
-    <mergeCell ref="B15:B22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1487,10 +1546,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD5444D-5353-498B-B134-3C7F6C4BB98B}">
-  <dimension ref="B2:P38"/>
+  <dimension ref="B2:P58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1533,10 +1592,10 @@
       <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="25"/>
+      <c r="G3" s="29"/>
       <c r="H3" s="2" t="s">
         <v>17</v>
       </c>
@@ -1595,23 +1654,23 @@
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
         <v>37</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
         <v>39</v>
-      </c>
-      <c r="G7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
@@ -1623,15 +1682,15 @@
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="21" t="s">
+      <c r="B10" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="25" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="23" t="s">
-        <v>47</v>
+      <c r="E10" s="24" t="s">
+        <v>45</v>
       </c>
       <c r="F10" t="s">
         <v>29</v>
@@ -1644,58 +1703,58 @@
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="23"/>
-      <c r="C11" s="21"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="25"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="23"/>
+      <c r="E11" s="24"/>
       <c r="F11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H11" t="s">
         <v>116</v>
       </c>
-      <c r="G11" t="s">
-        <v>117</v>
-      </c>
-      <c r="H11" t="s">
-        <v>118</v>
-      </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="23"/>
-      <c r="C12" s="21"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="23"/>
+      <c r="E12" s="24"/>
       <c r="F12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
         <v>39</v>
       </c>
-      <c r="G12" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="23"/>
-      <c r="C13" s="21"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="23"/>
+      <c r="E13" s="24"/>
       <c r="F13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" t="s">
         <v>40</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
         <v>44</v>
       </c>
-      <c r="H13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="23"/>
-      <c r="C14" s="21"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="23"/>
+      <c r="E14" s="24"/>
       <c r="F14" t="s">
         <v>20</v>
       </c>
@@ -1706,14 +1765,14 @@
         <v>19</v>
       </c>
       <c r="I14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B15" s="23"/>
-      <c r="C15" s="21"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="25"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="23"/>
+      <c r="E15" s="24"/>
       <c r="F15" t="s">
         <v>21</v>
       </c>
@@ -1725,105 +1784,112 @@
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C16" s="7"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="21"/>
       <c r="D16" s="3"/>
+      <c r="E16" s="22"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C17" s="17"/>
+      <c r="B17" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="18" t="s">
-        <v>101</v>
-      </c>
+      <c r="E17" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="22"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="22"/>
       <c r="F18" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="G18" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="H18" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="18"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="22"/>
       <c r="F19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="22"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="22"/>
+      <c r="F20" t="s">
         <v>20</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G20" t="s">
         <v>11</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="18"/>
-      <c r="F20" t="s">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="22"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="22"/>
+      <c r="F21" t="s">
         <v>21</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>12</v>
-      </c>
-      <c r="H20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="18"/>
-      <c r="F21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" t="s">
-        <v>25</v>
       </c>
       <c r="H21" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="18"/>
-      <c r="F22" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" t="s">
-        <v>26</v>
-      </c>
-      <c r="H22" t="s">
-        <v>22</v>
-      </c>
+      <c r="B22" s="22"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="22"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="9"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="2:8" ht="33" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>102</v>
+        <v>32</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F24" t="s">
         <v>29</v>
@@ -1835,21 +1901,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
       <c r="E25" s="18"/>
       <c r="F25" t="s">
-        <v>105</v>
+        <v>20</v>
       </c>
       <c r="G25" t="s">
-        <v>106</v>
+        <v>11</v>
       </c>
       <c r="H25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
       <c r="E26" s="18"/>
@@ -1892,120 +1958,398 @@
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
       <c r="E29" s="9"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>102</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="26" t="s">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="17"/>
+      <c r="E30" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="18"/>
+      <c r="F31" t="s">
+        <v>103</v>
+      </c>
+      <c r="G31" t="s">
         <v>104</v>
       </c>
-      <c r="F31" t="s">
-        <v>29</v>
-      </c>
-      <c r="G31" t="s">
-        <v>30</v>
-      </c>
       <c r="H31" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
-      <c r="E32" s="26"/>
+      <c r="E32" s="18"/>
       <c r="F32" t="s">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="G32" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="H32" t="s">
-        <v>107</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="E33" s="26"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="18"/>
       <c r="F33" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G33" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H33" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="E34" s="26"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="18"/>
       <c r="F34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G34" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H34" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="E35" s="26"/>
-      <c r="F35" t="s">
-        <v>24</v>
-      </c>
-      <c r="G35" t="s">
-        <v>26</v>
-      </c>
-      <c r="H35" t="s">
-        <v>22</v>
-      </c>
+      <c r="E35" s="9"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F37" t="s">
+        <v>29</v>
+      </c>
+      <c r="G37" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="30"/>
+      <c r="F38" t="s">
+        <v>103</v>
+      </c>
+      <c r="G38" t="s">
+        <v>104</v>
+      </c>
+      <c r="H38" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E39" s="30"/>
+      <c r="F39" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E40" s="30"/>
+      <c r="F40" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" t="s">
+        <v>25</v>
+      </c>
+      <c r="H40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E41" s="30"/>
+      <c r="F41" t="s">
+        <v>24</v>
+      </c>
+      <c r="G41" t="s">
+        <v>26</v>
+      </c>
+      <c r="H41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="23"/>
+    </row>
+    <row r="43" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="21"/>
+      <c r="E43" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="F43" t="s">
+        <v>128</v>
+      </c>
+      <c r="G43" t="s">
+        <v>136</v>
+      </c>
+      <c r="H43" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E44" s="28"/>
+      <c r="F44" t="s">
+        <v>37</v>
+      </c>
+      <c r="G44" t="s">
+        <v>41</v>
+      </c>
+      <c r="H44" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D45" s="21"/>
+      <c r="E45" s="28"/>
+      <c r="F45" t="s">
+        <v>38</v>
+      </c>
+      <c r="G45" t="s">
+        <v>42</v>
+      </c>
+      <c r="H45" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="28"/>
+      <c r="F46" t="s">
+        <v>20</v>
+      </c>
+      <c r="G46" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="28"/>
+      <c r="F47" t="s">
+        <v>21</v>
+      </c>
+      <c r="G47" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="28"/>
+      <c r="F48" t="s">
+        <v>129</v>
+      </c>
+      <c r="G48" t="s">
+        <v>131</v>
+      </c>
+      <c r="H48" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="23"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>130</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" s="21"/>
+      <c r="E50" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="F50" t="s">
+        <v>128</v>
+      </c>
+      <c r="G50" t="s">
+        <v>136</v>
+      </c>
+      <c r="H50" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="28"/>
+      <c r="F51" t="s">
+        <v>37</v>
+      </c>
+      <c r="G51" t="s">
+        <v>41</v>
+      </c>
+      <c r="H51" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="28"/>
+      <c r="F52" t="s">
+        <v>38</v>
+      </c>
+      <c r="G52" t="s">
+        <v>42</v>
+      </c>
+      <c r="H52" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="28"/>
+      <c r="F53" t="s">
+        <v>20</v>
+      </c>
+      <c r="G53" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="28"/>
+      <c r="F54" t="s">
+        <v>21</v>
+      </c>
+      <c r="G54" t="s">
+        <v>12</v>
+      </c>
+      <c r="H54" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="28"/>
+      <c r="F55" t="s">
+        <v>129</v>
+      </c>
+      <c r="G55" t="s">
+        <v>131</v>
+      </c>
+      <c r="H55" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="20"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E57" t="s">
+        <v>107</v>
+      </c>
+      <c r="F57" t="s">
         <v>108</v>
       </c>
-      <c r="C37" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="G57" t="s">
+        <v>110</v>
+      </c>
+      <c r="H57" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F58" t="s">
         <v>109</v>
       </c>
-      <c r="F37" t="s">
-        <v>110</v>
-      </c>
-      <c r="G37" t="s">
-        <v>112</v>
-      </c>
-      <c r="H37" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="F38" t="s">
+      <c r="G58" t="s">
         <v>111</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H58" t="s">
         <v>113</v>
       </c>
-      <c r="H38" t="s">
-        <v>115</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="E43:E48"/>
+    <mergeCell ref="E50:E55"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="E31:E35"/>
+    <mergeCell ref="E37:E41"/>
     <mergeCell ref="E10:E15"/>
     <mergeCell ref="C10:C15"/>
     <mergeCell ref="B10:B15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C11 C43:C1048576 C16:C35 C37" xr:uid="{57DF0A07-DFD1-4940-B876-132952E88629}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C11 C63:C1048576 C53:C57 C17:C20 C23:C43 C46:C50" xr:uid="{57DF0A07-DFD1-4940-B876-132952E88629}">
       <formula1>$D$4:$D$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>